<commit_message>
adjusting function to report properly
</commit_message>
<xml_diff>
--- a/Output/AllModels_final_with_plan_2000.xlsx
+++ b/Output/AllModels_final_with_plan_2000.xlsx
@@ -1,1186 +1,1193 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kueng\DataAnalysis\02TimeAndTiesControl_updatedBRMS\Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EA031C-A7CE-4BCB-95CA-F420E997C11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="387">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Subjective MVPA Hurdle Lognormal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device-Based MVPA Log (Gaussian)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mood Gaussian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactance Ordinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactance Dichotome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exp(Est.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95% CI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intercept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.92***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[32.74, 43.51]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111.05***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[99.57, 123.77]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.66***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 3.45, 3.87]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.34**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.17,   0.64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Intercept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.25***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.19,  0.35]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional Within-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.98,  1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.00,   1.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.04, 0.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.84*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.71,     0.98]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.68,   1.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.99,  1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.921</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.99,   1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.02, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.83,     1.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.84,   1.53]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.82,  1.00]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.88,   1.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.14, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.86*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  1.15,     2.72]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.96*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.01,   4.19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.86,  1.03]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.92,   1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.693</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.15, 0.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.69,     2.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.59,   4.29]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.795</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.92,  1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.96,   1.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.06, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.98,     1.53]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.33*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.03,   1.75]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.90,  1.02]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.96,   1.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.00, 0.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.974</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.71,     1.21]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.62,   1.34]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.679</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.88,  1.12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.91,   1.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.793</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.15, 0.36]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.75,     2.98]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.880</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.77,   3.72]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Own actionplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.33***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.21,  1.46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.06*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.02,   1.12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.10**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.02, 0.18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.48,     1.50]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.45,   1.66]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partner actionplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.99,  1.18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.00,   1.10]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.967</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.11, 0.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.56,     1.53]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.49,   1.56]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.00,   1.00]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.75,  1.40]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.84,   1.47]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.769</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.17, 0.90]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.902</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.38,     2.89]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.53,   7.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.848</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.71,  1.34]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.74,   1.32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.27, 0.80]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.43,     4.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.47,   7.53]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.84,  1.71]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.73,   1.31]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.85, 0.20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.54*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  1.32,    10.91]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.71**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[2.46, 165.20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.65,  1.34]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.631</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.74,   1.28]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.89, 0.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.38,     3.61]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.26,  19.62]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.764</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.76,  1.89]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.788</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.63,   1.47]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.56, 0.97]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.30,     6.19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.12,   6.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.549</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.80,  2.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.866</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.80,   1.85]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.842</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.39, 1.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.11*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.02,     0.66]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01,   0.72]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Within-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.58***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.39,  1.86]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.34***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.19,  1.54]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.70,  1.30]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.48*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.06,  2.28]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.71,  1.32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.29*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.05,  1.64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.65,  1.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Own actionplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.47***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 7.76, 11.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Partner actionplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.96,  1.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.67,  2.90]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.63,  2.75]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.40*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.17,  0.91]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.21,  1.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.40,  3.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.590</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.71,  5.56]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.909</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Random Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.23, 0.41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.23, 0.39]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.48, 0.78]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.46, 1.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.74, 1.78]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hurdle Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.56, 0.98]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.07, 0.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.10]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.52]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.04, 0.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.13, 0.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.22]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.08, 1.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.16, 2.39]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.26]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 1.55]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05, 2.69]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.52]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.63]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.16]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.62]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.97]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.03, 0.40]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.36]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.68]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.87]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.31, 0.98]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.55]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sigma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.65, 0.70]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.56, 0.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.94, 0.98]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="387">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Subjective MVPA Hurdle Lognormal</t>
+  </si>
+  <si>
+    <t>Device-Based MVPA Log (Gaussian)</t>
+  </si>
+  <si>
+    <t>Mood Gaussian</t>
+  </si>
+  <si>
+    <t>Reactance Ordinal</t>
+  </si>
+  <si>
+    <t>Reactance Dichotome</t>
+  </si>
+  <si>
+    <t>exp(Est.)</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>Est.</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>37.92***</t>
+  </si>
+  <si>
+    <t>[32.74, 43.51]</t>
+  </si>
+  <si>
+    <t>1.000</t>
+  </si>
+  <si>
+    <t>111.05***</t>
+  </si>
+  <si>
+    <t>[99.57, 123.77]</t>
+  </si>
+  <si>
+    <t>3.66***</t>
+  </si>
+  <si>
+    <t>[ 3.45, 3.87]</t>
+  </si>
+  <si>
+    <t>0.34**</t>
+  </si>
+  <si>
+    <t>[0.17,   0.64]</t>
+  </si>
+  <si>
+    <t>0.999</t>
+  </si>
+  <si>
+    <t>Hurdle Intercept</t>
+  </si>
+  <si>
+    <t>0.25***</t>
+  </si>
+  <si>
+    <t>[ 0.19,  0.35]</t>
+  </si>
+  <si>
+    <t>Conditional Within-Person Effects</t>
+  </si>
+  <si>
+    <t>Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>[ 0.98,  1.08]</t>
+  </si>
+  <si>
+    <t>0.855</t>
+  </si>
+  <si>
+    <t>[ 1.00,   1.06]</t>
+  </si>
+  <si>
+    <t>0.956</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>[-0.04, 0.05]</t>
+  </si>
+  <si>
+    <t>0.513</t>
+  </si>
+  <si>
+    <t>0.84*</t>
+  </si>
+  <si>
+    <t>[  0.71,     0.98]</t>
+  </si>
+  <si>
+    <t>0.985</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>[0.68,   1.01]</t>
+  </si>
+  <si>
+    <t>0.972</t>
+  </si>
+  <si>
+    <t>Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>[ 0.99,  1.08]</t>
+  </si>
+  <si>
+    <t>0.921</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>[ 0.99,   1.05]</t>
+  </si>
+  <si>
+    <t>0.876</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>[-0.02, 0.07]</t>
+  </si>
+  <si>
+    <t>0.817</t>
+  </si>
+  <si>
+    <t>[  0.83,     1.23]</t>
+  </si>
+  <si>
+    <t>0.592</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>[0.84,   1.53]</t>
+  </si>
+  <si>
+    <t>0.776</t>
+  </si>
+  <si>
+    <t>Daily pressure experienced</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>[ 0.82,  1.00]</t>
+  </si>
+  <si>
+    <t>0.971</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>[ 0.88,   1.01]</t>
+  </si>
+  <si>
+    <t>0.946</t>
+  </si>
+  <si>
+    <t>-0.03</t>
+  </si>
+  <si>
+    <t>[-0.14, 0.07]</t>
+  </si>
+  <si>
+    <t>0.718</t>
+  </si>
+  <si>
+    <t>1.86*</t>
+  </si>
+  <si>
+    <t>[  1.15,     2.72]</t>
+  </si>
+  <si>
+    <t>0.991</t>
+  </si>
+  <si>
+    <t>1.96*</t>
+  </si>
+  <si>
+    <t>[1.01,   4.19]</t>
+  </si>
+  <si>
+    <t>0.976</t>
+  </si>
+  <si>
+    <t>Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>[ 0.86,  1.03]</t>
+  </si>
+  <si>
+    <t>0.890</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>[ 0.92,   1.05]</t>
+  </si>
+  <si>
+    <t>0.693</t>
+  </si>
+  <si>
+    <t>[-0.15, 0.08]</t>
+  </si>
+  <si>
+    <t>0.691</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>[  0.69,     2.14]</t>
+  </si>
+  <si>
+    <t>0.808</t>
+  </si>
+  <si>
+    <t>1.42</t>
+  </si>
+  <si>
+    <t>[0.59,   4.29]</t>
+  </si>
+  <si>
+    <t>0.795</t>
+  </si>
+  <si>
+    <t>Daily pushing experienced</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>[ 0.92,  1.05]</t>
+  </si>
+  <si>
+    <t>0.666</t>
+  </si>
+  <si>
+    <t>[ 0.96,   1.06]</t>
+  </si>
+  <si>
+    <t>0.725</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>[-0.06, 0.07]</t>
+  </si>
+  <si>
+    <t>0.577</t>
+  </si>
+  <si>
+    <t>1.21</t>
+  </si>
+  <si>
+    <t>[  0.98,     1.53]</t>
+  </si>
+  <si>
+    <t>0.961</t>
+  </si>
+  <si>
+    <t>1.33*</t>
+  </si>
+  <si>
+    <t>[1.03,   1.75]</t>
+  </si>
+  <si>
+    <t>0.986</t>
+  </si>
+  <si>
+    <t>Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>[ 0.90,  1.02]</t>
+  </si>
+  <si>
+    <t>0.905</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>[ 0.96,   1.04]</t>
+  </si>
+  <si>
+    <t>0.517</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>[ 0.00, 0.14]</t>
+  </si>
+  <si>
+    <t>0.974</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>[  0.71,     1.21]</t>
+  </si>
+  <si>
+    <t>0.709</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>[0.62,   1.34]</t>
+  </si>
+  <si>
+    <t>0.679</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>[ 0.88,  1.12]</t>
+  </si>
+  <si>
+    <t>0.574</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>[ 0.91,   1.04]</t>
+  </si>
+  <si>
+    <t>0.793</t>
+  </si>
+  <si>
+    <t>0.26***</t>
+  </si>
+  <si>
+    <t>[ 0.15, 0.36]</t>
+  </si>
+  <si>
+    <t>1.49</t>
+  </si>
+  <si>
+    <t>[  0.75,     2.98]</t>
+  </si>
+  <si>
+    <t>0.880</t>
+  </si>
+  <si>
+    <t>1.67</t>
+  </si>
+  <si>
+    <t>[0.77,   3.72]</t>
+  </si>
+  <si>
+    <t>0.897</t>
+  </si>
+  <si>
+    <t>Own actionplan</t>
+  </si>
+  <si>
+    <t>1.33***</t>
+  </si>
+  <si>
+    <t>[ 1.21,  1.46]</t>
+  </si>
+  <si>
+    <t>1.06*</t>
+  </si>
+  <si>
+    <t>[ 1.02,   1.12]</t>
+  </si>
+  <si>
+    <t>0.995</t>
+  </si>
+  <si>
+    <t>0.10**</t>
+  </si>
+  <si>
+    <t>[ 0.02, 0.18]</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>[  0.48,     1.50]</t>
+  </si>
+  <si>
+    <t>0.701</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>[0.45,   1.66]</t>
+  </si>
+  <si>
+    <t>0.670</t>
+  </si>
+  <si>
+    <t>Partner actionplan</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>[ 0.99,  1.18]</t>
+  </si>
+  <si>
+    <t>0.959</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>[ 1.00,   1.10]</t>
+  </si>
+  <si>
+    <t>0.967</t>
+  </si>
+  <si>
+    <t>[-0.11, 0.04]</t>
+  </si>
+  <si>
+    <t>[  0.56,     1.53]</t>
+  </si>
+  <si>
+    <t>0.628</t>
+  </si>
+  <si>
+    <t>[0.49,   1.56]</t>
+  </si>
+  <si>
+    <t>Daily weartime</t>
+  </si>
+  <si>
+    <t>1.00***</t>
+  </si>
+  <si>
+    <t>[ 1.00,   1.00]</t>
+  </si>
+  <si>
+    <t>Conditional Between-Person Effects</t>
+  </si>
+  <si>
+    <t>Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t>[ 0.75,  1.40]</t>
+  </si>
+  <si>
+    <t>0.539</t>
+  </si>
+  <si>
+    <t>[ 0.84,   1.47]</t>
+  </si>
+  <si>
+    <t>0.769</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>[-0.17, 0.90]</t>
+  </si>
+  <si>
+    <t>0.902</t>
+  </si>
+  <si>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>[  0.38,     2.89]</t>
+  </si>
+  <si>
+    <t>0.550</t>
+  </si>
+  <si>
+    <t>1.90</t>
+  </si>
+  <si>
+    <t>[0.53,   7.06]</t>
+  </si>
+  <si>
+    <t>0.848</t>
+  </si>
+  <si>
+    <t>Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>[ 0.71,  1.34]</t>
+  </si>
+  <si>
+    <t>0.555</t>
+  </si>
+  <si>
+    <t>[ 0.74,   1.32]</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>[-0.27, 0.80]</t>
+  </si>
+  <si>
+    <t>0.814</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>[  0.43,     4.05]</t>
+  </si>
+  <si>
+    <t>1.81</t>
+  </si>
+  <si>
+    <t>[0.47,   7.53]</t>
+  </si>
+  <si>
+    <t>0.806</t>
+  </si>
+  <si>
+    <t>Mean pressure experienced</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>[ 0.84,  1.71]</t>
+  </si>
+  <si>
+    <t>0.824</t>
+  </si>
+  <si>
+    <t>[ 0.73,   1.31]</t>
+  </si>
+  <si>
+    <t>0.526</t>
+  </si>
+  <si>
+    <t>-0.33</t>
+  </si>
+  <si>
+    <t>[-0.85, 0.20]</t>
+  </si>
+  <si>
+    <t>0.882</t>
+  </si>
+  <si>
+    <t>3.54*</t>
+  </si>
+  <si>
+    <t>[  1.32,    10.91]</t>
+  </si>
+  <si>
+    <t>0.993</t>
+  </si>
+  <si>
+    <t>17.71**</t>
+  </si>
+  <si>
+    <t>[2.46, 165.20]</t>
+  </si>
+  <si>
+    <t>0.998</t>
+  </si>
+  <si>
+    <t>Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>[ 0.65,  1.34]</t>
+  </si>
+  <si>
+    <t>0.631</t>
+  </si>
+  <si>
+    <t>[ 0.74,   1.28]</t>
+  </si>
+  <si>
+    <t>0.570</t>
+  </si>
+  <si>
+    <t>-0.34</t>
+  </si>
+  <si>
+    <t>[-0.89, 0.17]</t>
+  </si>
+  <si>
+    <t>0.888</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>[  0.38,     3.61]</t>
+  </si>
+  <si>
+    <t>0.599</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>[0.26,  19.62]</t>
+  </si>
+  <si>
+    <t>0.764</t>
+  </si>
+  <si>
+    <t>Mean pushing experienced</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>[ 0.76,  1.89]</t>
+  </si>
+  <si>
+    <t>0.788</t>
+  </si>
+  <si>
+    <t>[ 0.63,   1.47]</t>
+  </si>
+  <si>
+    <t>0.615</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>[-0.56, 0.97]</t>
+  </si>
+  <si>
+    <t>0.706</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>[  0.30,     6.19]</t>
+  </si>
+  <si>
+    <t>0.630</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>[0.12,   6.09]</t>
+  </si>
+  <si>
+    <t>0.549</t>
+  </si>
+  <si>
+    <t>Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>[ 0.80,  2.07]</t>
+  </si>
+  <si>
+    <t>0.866</t>
+  </si>
+  <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>[ 0.80,   1.85]</t>
+  </si>
+  <si>
+    <t>0.842</t>
+  </si>
+  <si>
+    <t>[-0.39, 1.13]</t>
+  </si>
+  <si>
+    <t>0.836</t>
+  </si>
+  <si>
+    <t>0.11*</t>
+  </si>
+  <si>
+    <t>[  0.02,     0.66]</t>
+  </si>
+  <si>
+    <t>0.09*</t>
+  </si>
+  <si>
+    <t>[0.01,   0.72]</t>
+  </si>
+  <si>
+    <t>0.987</t>
+  </si>
+  <si>
+    <t>Mean weartime</t>
+  </si>
+  <si>
+    <t>0.914</t>
+  </si>
+  <si>
+    <t>Hurdle Within-Person Effects</t>
+  </si>
+  <si>
+    <t>Hu Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t>1.58***</t>
+  </si>
+  <si>
+    <t>[ 1.39,  1.86]</t>
+  </si>
+  <si>
+    <t>Hu Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>1.34***</t>
+  </si>
+  <si>
+    <t>[ 1.19,  1.54]</t>
+  </si>
+  <si>
+    <t>Hu Daily pressure experienced</t>
+  </si>
+  <si>
+    <t>[ 0.70,  1.30]</t>
+  </si>
+  <si>
+    <t>0.625</t>
+  </si>
+  <si>
+    <t>Hu Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>1.48*</t>
+  </si>
+  <si>
+    <t>[ 1.06,  2.28]</t>
+  </si>
+  <si>
+    <t>0.990</t>
+  </si>
+  <si>
+    <t>Hu Daily pushing experienced</t>
+  </si>
+  <si>
+    <t>[ 0.71,  1.32]</t>
+  </si>
+  <si>
+    <t>0.633</t>
+  </si>
+  <si>
+    <t>Hu Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>1.29*</t>
+  </si>
+  <si>
+    <t>[ 1.05,  1.64]</t>
+  </si>
+  <si>
+    <t>0.992</t>
+  </si>
+  <si>
+    <t>Hu Day</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>[ 0.65,  1.15]</t>
+  </si>
+  <si>
+    <t>0.854</t>
+  </si>
+  <si>
+    <t>Hu Own actionplan</t>
+  </si>
+  <si>
+    <t>9.47***</t>
+  </si>
+  <si>
+    <t>[ 7.76, 11.59]</t>
+  </si>
+  <si>
+    <t>Hu Partner actionplan</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>[ 0.96,  1.42]</t>
+  </si>
+  <si>
+    <t>0.938</t>
+  </si>
+  <si>
+    <t>Hu Daily weartime</t>
+  </si>
+  <si>
+    <t>Hurdle Between-Person Effects</t>
+  </si>
+  <si>
+    <t>Hu Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>[ 0.67,  2.90]</t>
+  </si>
+  <si>
+    <t>0.831</t>
+  </si>
+  <si>
+    <t>Hu Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>[ 0.63,  2.75]</t>
+  </si>
+  <si>
+    <t>Hu Mean pressure experienced</t>
+  </si>
+  <si>
+    <t>0.40*</t>
+  </si>
+  <si>
+    <t>[ 0.17,  0.91]</t>
+  </si>
+  <si>
+    <t>Hu Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>[ 0.21,  1.17]</t>
+  </si>
+  <si>
+    <t>0.942</t>
+  </si>
+  <si>
+    <t>Hu Mean pushing experienced</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>[ 0.40,  3.17]</t>
+  </si>
+  <si>
+    <t>0.590</t>
+  </si>
+  <si>
+    <t>Hu Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>[ 0.71,  5.56]</t>
+  </si>
+  <si>
+    <t>0.909</t>
+  </si>
+  <si>
+    <t>Hu Mean weartime</t>
+  </si>
+  <si>
+    <t>Random Effects</t>
+  </si>
+  <si>
+    <t>sd(Intercept)</t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>[0.23, 0.41]</t>
+  </si>
+  <si>
+    <t>[0.23, 0.39]</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>[0.48, 0.78]</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>[0.46, 1.27]</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>[0.74, 1.78]</t>
+  </si>
+  <si>
+    <t>sd(Hurdle Intercept)</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>[0.56, 0.98]</t>
+  </si>
+  <si>
+    <t>sd(Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t>0.11</t>
+  </si>
+  <si>
+    <t>[0.07, 0.17]</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>[0.02, 0.08]</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>[0.00, 0.10]</t>
+  </si>
+  <si>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>[0.01, 0.42]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.52]</t>
+  </si>
+  <si>
+    <t>sd(Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>[0.04, 0.13]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.09]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.13]</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>[0.13, 0.99]</t>
+  </si>
+  <si>
+    <t>sd(Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>[0.00, 0.22]</t>
+  </si>
+  <si>
+    <t>[0.00, 0.13]</t>
+  </si>
+  <si>
+    <t>[0.00, 0.23]</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>[0.08, 1.17]</t>
+  </si>
+  <si>
+    <t>[0.16, 2.39]</t>
+  </si>
+  <si>
+    <t>sd(Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>[0.00, 0.18]</t>
+  </si>
+  <si>
+    <t>[0.00, 0.11]</t>
+  </si>
+  <si>
+    <t>[0.00, 0.26]</t>
+  </si>
+  <si>
+    <t>0.40</t>
+  </si>
+  <si>
+    <t>[0.02, 1.55]</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>[0.05, 2.69]</t>
+  </si>
+  <si>
+    <t>sd(Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>[0.01, 0.17]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.15]</t>
+  </si>
+  <si>
+    <t>[0.00, 0.15]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.52]</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>[0.01, 0.63]</t>
+  </si>
+  <si>
+    <t>sd(Daily pushing utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>[0.00, 0.16]</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>[0.01, 0.62]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.97]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t>[0.03, 0.40]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>[0.01, 0.36]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t>[0.01, 0.68]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>[0.01, 0.87]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>[0.31, 0.98]</t>
+  </si>
+  <si>
+    <t>sd(Hu Daily pushing utilized (partner's view))</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>[0.02, 0.55]</t>
+  </si>
+  <si>
+    <t>Additional Parameters</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>[0.65, 0.70]</t>
+  </si>
+  <si>
+    <t>[0.56, 0.59]</t>
+  </si>
+  <si>
+    <t>[0.94, 0.98]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1194,16 +1201,16 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <i/>
     </font>
   </fonts>
   <fills count="2">
@@ -1223,20 +1230,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1252,20 +1267,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1547,64 +1577,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="40.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.2265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.2265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.2265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.2265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.2265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +1704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1698,7 +1748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1724,58 +1774,58 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1824,8 +1874,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1874,8 +1924,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A8" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1924,8 +1974,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A9" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1974,8 +2024,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2024,8 +2074,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A11" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2074,8 +2124,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A12" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2124,8 +2174,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A13" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2174,8 +2224,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A14" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2224,8 +2274,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A15" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B15" s="1"/>
@@ -2250,58 +2300,58 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A16" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A17" s="7" t="s">
         <v>160</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2350,8 +2400,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A18" s="7" t="s">
         <v>174</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2400,8 +2450,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A19" s="7" t="s">
         <v>186</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2450,8 +2500,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A20" s="7" t="s">
         <v>201</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2500,8 +2550,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A21" s="7" t="s">
         <v>216</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2550,8 +2600,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A22" s="7" t="s">
         <v>231</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2600,8 +2650,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A23" s="7" t="s">
         <v>245</v>
       </c>
       <c r="B23" s="1"/>
@@ -2626,58 +2676,58 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A24" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="P24" s="11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A25" s="7" t="s">
         <v>248</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2702,8 +2752,8 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A26" s="7" t="s">
         <v>251</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2728,8 +2778,8 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A27" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2754,8 +2804,8 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A28" s="7" t="s">
         <v>257</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2780,8 +2830,8 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A29" s="7" t="s">
         <v>261</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2806,8 +2856,8 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A30" s="7" t="s">
         <v>264</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -2832,8 +2882,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A31" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2858,8 +2908,8 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A32" s="7" t="s">
         <v>272</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -2884,8 +2934,8 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A33" s="7" t="s">
         <v>275</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2910,8 +2960,8 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A34" s="7" t="s">
         <v>279</v>
       </c>
       <c r="B34" s="1"/>
@@ -2930,58 +2980,58 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A35" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="M35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="N35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="O35" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="P35" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A36" s="7" t="s">
         <v>281</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -3006,8 +3056,8 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A37" s="7" t="s">
         <v>285</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3032,8 +3082,8 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A38" s="7" t="s">
         <v>288</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -3058,8 +3108,8 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A39" s="7" t="s">
         <v>291</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -3084,8 +3134,8 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40">
-      <c r="A40" s="8" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A40" s="7" t="s">
         <v>295</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -3110,8 +3160,8 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A41" s="7" t="s">
         <v>299</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3136,8 +3186,8 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A42" s="7" t="s">
         <v>303</v>
       </c>
       <c r="B42" s="1"/>
@@ -3156,58 +3206,58 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A43" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="L43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="M43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="N43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="O43" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="P43" s="11" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A44" s="7" t="s">
         <v>305</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3246,8 +3296,8 @@
       </c>
       <c r="P44" s="1"/>
     </row>
-    <row r="45">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A45" s="7" t="s">
         <v>315</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3270,8 +3320,8 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A46" s="7" t="s">
         <v>318</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -3310,8 +3360,8 @@
       </c>
       <c r="P46" s="1"/>
     </row>
-    <row r="47">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A47" s="7" t="s">
         <v>328</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3350,8 +3400,8 @@
       </c>
       <c r="P47" s="1"/>
     </row>
-    <row r="48">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A48" s="7" t="s">
         <v>335</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -3390,8 +3440,8 @@
       </c>
       <c r="P48" s="1"/>
     </row>
-    <row r="49">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A49" s="7" t="s">
         <v>343</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3430,8 +3480,8 @@
       </c>
       <c r="P49" s="1"/>
     </row>
-    <row r="50">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A50" s="7" t="s">
         <v>351</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -3470,8 +3520,8 @@
       </c>
       <c r="P50" s="1"/>
     </row>
-    <row r="51">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A51" s="7" t="s">
         <v>359</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3510,8 +3560,8 @@
       </c>
       <c r="P51" s="1"/>
     </row>
-    <row r="52">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A52" s="7" t="s">
         <v>365</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -3534,8 +3584,8 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A53" s="7" t="s">
         <v>367</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -3558,8 +3608,8 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54">
-      <c r="A54" s="8" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A54" s="7" t="s">
         <v>370</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -3582,8 +3632,8 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55">
-      <c r="A55" s="8" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A55" s="7" t="s">
         <v>372</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -3606,8 +3656,8 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A56" s="7" t="s">
         <v>375</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -3630,8 +3680,8 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A57" s="7" t="s">
         <v>378</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -3654,58 +3704,58 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A58" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="I58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="J58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="K58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="L58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="M58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="N58" s="1" t="s">
+      <c r="N58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="O58" s="1" t="s">
+      <c r="O58" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="P58" s="1" t="s">
+      <c r="P58" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A59" s="8" t="s">
         <v>382</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -3736,60 +3786,60 @@
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
     </row>
-    <row r="60">
-      <c r="A60" s="8"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="8"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="8"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="8"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="8"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="8"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="8"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="8"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="8"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="8"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="8"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="8"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="8"/>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A66" s="7"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A68" s="7"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A72" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A16:P16"/>
+    <mergeCell ref="A24:P24"/>
+    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="A43:P43"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A16:P16"/>
-    <mergeCell ref="A24:P24"/>
-    <mergeCell ref="A35:P35"/>
-    <mergeCell ref="A43:P43"/>
-    <mergeCell ref="A58:P58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>